<commit_message>
updated offscreen production without repeated games
</commit_message>
<xml_diff>
--- a/results and supplementary.xlsx
+++ b/results and supplementary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmm2651/Documents/cogslab/DigitEyes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD3E21-9E77-CB4F-9DAF-5B12AAEFA8AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92E3DCD-45E1-9540-875C-BEE4CCD3E78E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="17540" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16620" windowHeight="17540" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -48,6 +48,7 @@
             <sz val="11"/>
             <color indexed="8"/>
             <rFont val="Helvetica Neue"/>
+            <family val="2"/>
           </rPr>
           <t>Caitlyn McColeman:
 This is based on the data that was flagged as being in time stamps</t>
@@ -394,18 +395,9 @@
     <t>League 2 vs 6 (overall)</t>
   </si>
   <si>
-    <t>W = 75598</t>
-  </si>
-  <si>
-    <t>p-value = 4.421e-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Omnibus test </t>
   </si>
   <si>
-    <t>Kruskal-Wallis chi-squared = 164.33</t>
-  </si>
-  <si>
     <t xml:space="preserve">Novice/expert difference by race (League 2 vs 6) </t>
   </si>
   <si>
@@ -421,21 +413,9 @@
     <t>Terran</t>
   </si>
   <si>
-    <t>W = 6764.5</t>
-  </si>
-  <si>
-    <t>p-value = 0.002101</t>
-  </si>
-  <si>
     <t>Protoss</t>
   </si>
   <si>
-    <t>W = 9371.5</t>
-  </si>
-  <si>
-    <t>p-value = 1.703e-05</t>
-  </si>
-  <si>
     <t>betweenFixationAmplitude</t>
   </si>
   <si>
@@ -449,6 +429,27 @@
   </si>
   <si>
     <t>Kruskal-Wallis chi-squared = 336.82</t>
+  </si>
+  <si>
+    <t>W = 75242</t>
+  </si>
+  <si>
+    <t>p-value = 9.912e-14</t>
+  </si>
+  <si>
+    <t>Kruskal-Wallis chi-squared = 162.31</t>
+  </si>
+  <si>
+    <t>W = 6711.5</t>
+  </si>
+  <si>
+    <t>p-value = 0.003725</t>
+  </si>
+  <si>
+    <t>W = 9329.5</t>
+  </si>
+  <si>
+    <t>p-value = 2.239e-05</t>
   </si>
 </sst>
 </file>
@@ -479,28 +480,33 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -554,7 +560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -667,13 +673,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -884,6 +996,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -905,19 +1032,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2090,11 +2232,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -2349,7 +2491,7 @@
     </row>
     <row r="39" spans="2:4" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2357,10 +2499,10 @@
     <row r="40" spans="2:4" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2408,15 +2550,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
@@ -2657,11 +2799,11 @@
   </sheetPr>
   <dimension ref="A1:IV14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2670,15 +2812,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -2925,15 +3067,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -2946,10 +3088,10 @@
     </row>
     <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="61"/>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -2981,10 +3123,10 @@
     </row>
     <row r="6" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22"/>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="74"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -3052,15 +3194,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:7" s="67" customFormat="1" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="A1" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -3080,19 +3222,19 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="28" x14ac:dyDescent="0.15">
-      <c r="A3" s="77">
+      <c r="A3" s="70">
         <v>1</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="71">
         <v>-0.51224259999999999</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="71">
         <v>327.07977</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="72">
         <v>0.60882700000000001</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="71">
         <v>4.8312609999999999E-2</v>
       </c>
       <c r="F3" s="59"/>
@@ -3101,19 +3243,19 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="77">
+      <c r="A4" s="70">
         <v>2</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="71">
         <v>-3.1646728</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="71">
         <v>294.87808000000001</v>
       </c>
-      <c r="D4" s="79">
+      <c r="D4" s="72">
         <v>1.7148370000000001E-3</v>
       </c>
-      <c r="E4" s="78">
+      <c r="E4" s="71">
         <v>0.26805803</v>
       </c>
       <c r="F4" s="19"/>
@@ -3122,19 +3264,19 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="28" x14ac:dyDescent="0.15">
-      <c r="A5" s="77">
+      <c r="A5" s="70">
         <v>3</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="71">
         <v>-5.8308703</v>
       </c>
-      <c r="C5" s="78">
+      <c r="C5" s="71">
         <v>268.69529</v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="72">
         <v>1.5779259999999999E-8</v>
       </c>
-      <c r="E5" s="78">
+      <c r="E5" s="71">
         <v>0.44807385999999999</v>
       </c>
       <c r="F5" s="19"/>
@@ -3143,19 +3285,19 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="28" x14ac:dyDescent="0.15">
-      <c r="A6" s="77">
+      <c r="A6" s="70">
         <v>4</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="71">
         <v>-8.6722742999999998</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="71">
         <v>272.18335000000002</v>
       </c>
-      <c r="D6" s="79">
+      <c r="D6" s="72">
         <v>3.8980450000000002E-16</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="71">
         <v>0.66053768000000002</v>
       </c>
       <c r="F6" s="19"/>
@@ -3164,19 +3306,19 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="28" x14ac:dyDescent="0.15">
-      <c r="A7" s="77">
+      <c r="A7" s="70">
         <v>5</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="71">
         <v>-11.05691</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="71">
         <v>337.20414</v>
       </c>
-      <c r="D7" s="79">
+      <c r="D7" s="72">
         <v>1.8590680000000001E-24</v>
       </c>
-      <c r="E7" s="78">
+      <c r="E7" s="71">
         <v>0.83004522999999997</v>
       </c>
       <c r="F7" s="19"/>
@@ -3185,19 +3327,19 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="28" x14ac:dyDescent="0.15">
-      <c r="A8" s="77">
+      <c r="A8" s="70">
         <v>6</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="71">
         <v>-4.8170533999999998</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="71">
         <v>37.615839999999999</v>
       </c>
-      <c r="D8" s="79">
+      <c r="D8" s="72">
         <v>2.3964429999999999E-5</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E8" s="71">
         <v>1.09243651</v>
       </c>
       <c r="F8" s="19"/>
@@ -3227,11 +3369,11 @@
     </row>
     <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="22"/>
-      <c r="B11" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="81" t="s">
-        <v>128</v>
+      <c r="B11" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="74" t="s">
+        <v>121</v>
       </c>
       <c r="D11" s="69"/>
       <c r="E11" s="69"/>
@@ -3261,7 +3403,7 @@
     <row r="14" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="22"/>
       <c r="B14" s="68" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>23</v>
@@ -3301,15 +3443,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -3560,15 +3702,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -3819,15 +3961,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -4065,11 +4207,11 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4078,174 +4220,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="87" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8">
+      <c r="A3" s="82">
         <v>1</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="90">
         <v>-3.3493580000000001</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="90">
         <v>356.60523999999998</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="91">
         <v>8.9652769999999996E-4</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="90">
         <v>0.30537720000000002</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15">
+      <c r="A4" s="83">
         <v>2</v>
       </c>
-      <c r="B4" s="16">
-        <v>-4.7099770000000003</v>
-      </c>
-      <c r="C4" s="43">
-        <v>316.07405</v>
-      </c>
-      <c r="D4" s="18">
-        <v>3.7154769999999998E-6</v>
-      </c>
-      <c r="E4" s="19">
-        <v>0.38343329999999998</v>
-      </c>
-      <c r="F4" s="19"/>
+      <c r="B4" s="90">
+        <v>-4.6819600000000001</v>
+      </c>
+      <c r="C4" s="90">
+        <v>316.21859000000001</v>
+      </c>
+      <c r="D4" s="91">
+        <v>4.2226059999999998E-6</v>
+      </c>
+      <c r="E4" s="90">
+        <v>0.38134249999999997</v>
+      </c>
+      <c r="F4" s="85"/>
       <c r="G4" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15">
+      <c r="A5" s="83">
         <v>3</v>
       </c>
-      <c r="B5" s="16">
-        <v>-6.2936480000000001</v>
-      </c>
-      <c r="C5" s="43">
-        <v>254.85055</v>
-      </c>
-      <c r="D5" s="18">
-        <v>1.345391E-9</v>
-      </c>
-      <c r="E5" s="44">
-        <v>0.50577499999999997</v>
-      </c>
-      <c r="F5" s="44"/>
+      <c r="B5" s="90">
+        <v>-6.2728320000000002</v>
+      </c>
+      <c r="C5" s="90">
+        <v>254.87915000000001</v>
+      </c>
+      <c r="D5" s="91">
+        <v>1.5105999999999999E-9</v>
+      </c>
+      <c r="E5" s="90">
+        <v>0.50431979999999998</v>
+      </c>
+      <c r="F5" s="86"/>
       <c r="G5" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15">
+      <c r="A6" s="83">
         <v>4</v>
       </c>
-      <c r="B6" s="16">
-        <v>-9.1539239999999999</v>
-      </c>
-      <c r="C6" s="43">
-        <v>261.40591999999998</v>
-      </c>
-      <c r="D6" s="54">
-        <v>1.6299400000000001E-17</v>
-      </c>
-      <c r="E6" s="19">
-        <v>0.72054629999999997</v>
-      </c>
-      <c r="F6" s="19"/>
+      <c r="B6" s="90">
+        <v>-9.1436569999999993</v>
+      </c>
+      <c r="C6" s="90">
+        <v>261.89864999999998</v>
+      </c>
+      <c r="D6" s="91">
+        <v>1.7360879999999999E-17</v>
+      </c>
+      <c r="E6" s="90">
+        <v>0.71938670000000005</v>
+      </c>
+      <c r="F6" s="85"/>
       <c r="G6" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15">
+      <c r="A7" s="83">
         <v>5</v>
       </c>
-      <c r="B7" s="16">
-        <v>-9.8911940000000005</v>
-      </c>
-      <c r="C7" s="43">
-        <v>288.64961</v>
-      </c>
-      <c r="D7" s="18">
-        <v>4.682607E-20</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0.80949709999999997</v>
-      </c>
-      <c r="F7" s="19"/>
+      <c r="B7" s="90">
+        <v>-9.7785609999999998</v>
+      </c>
+      <c r="C7" s="90">
+        <v>288.33589999999998</v>
+      </c>
+      <c r="D7" s="91">
+        <v>1.089052E-19</v>
+      </c>
+      <c r="E7" s="90">
+        <v>0.80404109999999995</v>
+      </c>
+      <c r="F7" s="85"/>
       <c r="G7" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15">
+      <c r="A8" s="83">
         <v>6</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="90">
         <v>-7.043939</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="90">
         <v>45.524439999999998</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="91">
         <v>8.2605149999999996E-9</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="90">
         <v>1.3025749</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22"/>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -4255,11 +4397,11 @@
       <c r="A11" s="24">
         <v>7</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>112</v>
+      <c r="B11" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="74" t="s">
+        <v>124</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
@@ -4278,7 +4420,7 @@
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="22"/>
       <c r="B13" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -4290,8 +4432,8 @@
       <c r="A14" s="24">
         <v>8</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>114</v>
+      <c r="B14" s="73" t="s">
+        <v>125</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>23</v>
@@ -4300,7 +4442,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="26">
-        <v>4.7849719999999998E-2</v>
+        <v>4.738237E-2</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -4316,11 +4458,11 @@
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="22"/>
-      <c r="B16" s="73" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
+      <c r="B16" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -4328,7 +4470,7 @@
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="22"/>
       <c r="B17" s="25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -4341,10 +4483,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -4354,7 +4496,7 @@
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="22"/>
       <c r="B19" s="25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -4366,11 +4508,11 @@
       <c r="A20" s="24">
         <v>10</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>121</v>
+      <c r="B20" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>127</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -4380,7 +4522,7 @@
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="22"/>
       <c r="B21" s="25" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
@@ -4392,11 +4534,11 @@
       <c r="A22" s="24">
         <v>11</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>124</v>
+      <c r="B22" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>129</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -4437,15 +4579,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
@@ -4698,15 +4840,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -4968,15 +5110,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
@@ -5229,15 +5371,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -5497,15 +5639,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -5756,15 +5898,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -6015,15 +6157,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>
@@ -6283,15 +6425,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7"/>

</xml_diff>